<commit_message>
MvSR ka placment thik kiya
</commit_message>
<xml_diff>
--- a/Files/college_info/all_colleges/MVSR/MVSR_placements.xlsx
+++ b/Files/college_info/all_colleges/MVSR/MVSR_placements.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\91703\Desktop\gitt\PYTHON PROJECT\github\python_project-dataset\Files\college_info\all_colleges\MVSR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E15BC98-58BF-4C3A-9D76-AE6F6D1099CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3407ED37-9981-4DAA-8788-685158AC015E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <r>
       <rPr>
@@ -44,17 +44,6 @@
         <family val="2"/>
       </rPr>
       <t>Hexaware_GET</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <color rgb="FF233F62"/>
-        <rFont val="Trebuchet MS"/>
-        <family val="2"/>
-      </rPr>
-      <t>Nil</t>
     </r>
   </si>
   <si>
@@ -1238,7 +1227,7 @@
   <dimension ref="A1:D60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -1251,16 +1240,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="25.5" customHeight="1">
       <c r="A1" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="C1" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="C1" s="18" t="s">
+      <c r="D1" s="18" t="s">
         <v>55</v>
-      </c>
-      <c r="D1" s="18" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="21" customHeight="1">
@@ -1268,7 +1257,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="3">
         <v>14.95</v>
@@ -1282,13 +1271,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="3">
         <v>8</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>2</v>
+      <c r="D3" s="4">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="21" customHeight="1">
@@ -1296,7 +1285,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="3">
         <v>8</v>
@@ -1310,7 +1299,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5" s="3">
         <v>7.6</v>
@@ -1324,7 +1313,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3">
         <v>7.5</v>
@@ -1338,7 +1327,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="3">
         <v>7.2</v>
@@ -1352,7 +1341,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="3">
         <v>7.2</v>
@@ -1366,7 +1355,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9" s="4">
         <v>7</v>
@@ -1380,7 +1369,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C10" s="3">
         <v>7</v>
@@ -1394,7 +1383,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3">
         <v>6.89</v>
@@ -1408,7 +1397,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C12" s="3">
         <v>6.5</v>
@@ -1422,7 +1411,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="3">
         <v>6</v>
@@ -1436,7 +1425,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14" s="3">
         <v>6</v>
@@ -1450,7 +1439,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C15" s="3">
         <v>6</v>
@@ -1464,7 +1453,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="3">
         <v>5.5</v>
@@ -1478,7 +1467,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C17" s="3">
         <v>5</v>
@@ -1492,7 +1481,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" s="3">
         <v>5</v>
@@ -1506,7 +1495,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="3">
         <v>5</v>
@@ -1520,7 +1509,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C20" s="3">
         <v>5</v>
@@ -1534,7 +1523,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="3">
         <v>5</v>
@@ -1548,7 +1537,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C22" s="14">
         <v>5</v>
@@ -1562,7 +1551,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C23" s="3">
         <v>5</v>
@@ -1576,7 +1565,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C24" s="3">
         <v>4.75</v>
@@ -1590,7 +1579,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" s="3">
         <v>4.5</v>
@@ -1604,7 +1593,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C26" s="3">
         <v>4.5</v>
@@ -1618,7 +1607,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C27" s="14">
         <v>4.5</v>
@@ -1632,7 +1621,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" s="3">
         <v>4.5</v>
@@ -1646,7 +1635,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C29" s="3">
         <v>4.4000000000000004</v>
@@ -1660,7 +1649,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C30" s="3">
         <v>4.25</v>
@@ -1674,7 +1663,7 @@
         <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C31" s="3">
         <v>4.2</v>
@@ -1702,7 +1691,7 @@
         <v>32</v>
       </c>
       <c r="B33" s="12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33" s="13">
         <v>4</v>
@@ -1716,7 +1705,7 @@
         <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C34" s="3">
         <v>4</v>
@@ -1730,7 +1719,7 @@
         <v>34</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C35" s="3">
         <v>4</v>
@@ -1744,7 +1733,7 @@
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C36" s="3">
         <v>4</v>
@@ -1758,7 +1747,7 @@
         <v>36</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" s="3">
         <v>4</v>
@@ -1772,7 +1761,7 @@
         <v>37</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38" s="3">
         <v>4</v>
@@ -1786,7 +1775,7 @@
         <v>38</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C39" s="3">
         <v>4</v>
@@ -1800,7 +1789,7 @@
         <v>39</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C40" s="3">
         <v>4</v>
@@ -1814,7 +1803,7 @@
         <v>40</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C41" s="3">
         <v>4</v>
@@ -1828,7 +1817,7 @@
         <v>41</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C42" s="3">
         <v>3.6</v>
@@ -1842,7 +1831,7 @@
         <v>42</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C43" s="3">
         <v>3.6</v>
@@ -1856,7 +1845,7 @@
         <v>43</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C44" s="3">
         <v>3.6</v>
@@ -1870,7 +1859,7 @@
         <v>44</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C45" s="3">
         <v>3.6</v>
@@ -1884,7 +1873,7 @@
         <v>45</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C46" s="3">
         <v>3.6</v>
@@ -1912,7 +1901,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C48" s="3">
         <v>3.5</v>
@@ -1926,7 +1915,7 @@
         <v>48</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C49" s="3">
         <v>3.5</v>
@@ -1940,7 +1929,7 @@
         <v>49</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C50" s="3">
         <v>3.5</v>
@@ -1954,7 +1943,7 @@
         <v>50</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C51" s="3">
         <v>3.5</v>
@@ -1968,7 +1957,7 @@
         <v>51</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C52" s="3">
         <v>3.5</v>
@@ -1982,7 +1971,7 @@
         <v>52</v>
       </c>
       <c r="B53" s="20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C53" s="3">
         <v>3.5</v>
@@ -1996,7 +1985,7 @@
         <v>53</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C54" s="3">
         <v>3.5</v>
@@ -2010,7 +1999,7 @@
         <v>54</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C55" s="3">
         <v>3.4</v>
@@ -2024,7 +2013,7 @@
         <v>55</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C56" s="3">
         <v>3.36</v>
@@ -2038,7 +2027,7 @@
         <v>56</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C57" s="3">
         <v>3.36</v>
@@ -2052,7 +2041,7 @@
         <v>57</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C58" s="3">
         <v>3.36</v>
@@ -2066,7 +2055,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C59" s="3">
         <v>3.06</v>

</xml_diff>